<commit_message>
Reading all question and response data from Excel datafile.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katri\PythonProjects\quiz-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1087AC16-93A7-4C02-B7CD-798E77815889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C9387A-9B86-43B4-857C-0D566E37B923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{84DE1469-F088-4B7E-B0B1-260C4445CC6C}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>question_content</t>
   </si>
   <si>
-    <t>queston_rank</t>
-  </si>
-  <si>
     <t>response_content</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Cinema quiz</t>
+  </si>
+  <si>
+    <t>question_rank</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,16 +514,16 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -531,22 +531,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -554,22 +554,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -577,22 +577,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -600,22 +600,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -623,22 +623,22 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -646,22 +646,22 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -669,22 +669,22 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -692,22 +692,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -715,91 +715,91 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>26</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
         <v>29</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>